<commit_message>
Reformatted csv and json
</commit_message>
<xml_diff>
--- a/MilitaryBases.xlsx
+++ b/MilitaryBases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshs\Documents\Arsh Files on PC\Virginia Tech\Year 1\Semester 2\Clubs\WebDVT\HTML\html-cheat-sheet\TheSunNeverSetsOnTheAmericanMilitaryBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A36D34C-D0D6-4801-A422-8CB34CF5D6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD68627-5863-4756-943C-5E96F29AC61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="834" yWindow="-96" windowWidth="22302" windowHeight="14592" xr2:uid="{E398A702-D2C5-4257-8B81-705240FEDC0C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="223">
   <si>
     <t>NG Springfield AVCRAD (New)</t>
   </si>
@@ -701,6 +701,9 @@
   </si>
   <si>
     <t>long</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -1065,2369 +1068,2873 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCADE206-E22A-485D-8E8A-6C74ACC938AD}">
-  <dimension ref="A1:D168"/>
+  <dimension ref="A1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.89453125" customWidth="1"/>
-    <col min="2" max="2" width="24.578125" customWidth="1"/>
-    <col min="3" max="3" width="24.1015625" customWidth="1"/>
-    <col min="4" max="4" width="41.3671875" customWidth="1"/>
+    <col min="2" max="2" width="19.89453125" customWidth="1"/>
+    <col min="3" max="3" width="24.578125" customWidth="1"/>
+    <col min="4" max="4" width="24.1015625" customWidth="1"/>
+    <col min="5" max="5" width="41.3671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
         <v>208</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>209</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>220</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>37.253275482799999</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>-93.3909578934</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>61.603050334499997</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>-149.37484979000001</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>44.714336076000002</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>-123.270695898</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>21.318991725099998</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>-158.062484829</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>21.373515268399998</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>-157.93798769099999</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>21.338877742800001</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>-157.995139279</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>36.243764679000002</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>-119.883529044</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>30.972527677199999</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>-83.1646930406</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>31.386319091699999</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>-85.972271649099994</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>31.2285844723</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>-85.558709471699999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>21.495603491200001</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>-158.05323976599999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>40.6089967598</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>-74.029450058899997</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>40.792002592599999</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>-91.245615802100005</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>34.692850559999997</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>-77.028682555700001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>40.253857197999999</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>-74.160848341100007</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>36.925015289299999</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>-76.299610968400003</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>40.041303072200002</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>-75.094581271999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>13.4286325755</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>144.653464077</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>32.553191412300002</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>-88.569513127199997</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>35.331424226499998</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>-89.870783795099996</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D22" s="1">
         <v>30.575937619600001</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>-86.528373348599999</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D23" s="1">
         <v>41.934994050599997</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>-72.701250409400004</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D24" s="1">
         <v>39.686509694599998</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>-75.597556218600005</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D25" s="1">
         <v>43.0890854907</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>-70.818730765699996</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D26" s="1">
         <v>32.126420385899998</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>-81.189756560399999</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D27" s="1">
         <v>27.843608365400002</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>-82.501022748400004</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28" s="1">
         <v>36.891519218699997</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>-90.279966518400002</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29" s="1">
         <v>44.747748483099997</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>-93.127605437499994</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30" s="1">
         <v>32.838556947100003</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>-115.258177991</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="1">
+      <c r="D31" s="1">
         <v>29.9488308912</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>-90.0328996808</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
         <v>30.5080389773</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>-87.647194632199998</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33" s="1">
         <v>13.535862679799999</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>144.91480443500001</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="1">
+      <c r="D34" s="1">
         <v>33.984552387000001</v>
       </c>
-      <c r="D34" s="1">
+      <c r="E34" s="1">
         <v>-98.499693681799997</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="1">
+      <c r="D35" s="1">
         <v>48.189600582799997</v>
       </c>
-      <c r="D35" s="1">
+      <c r="E35" s="1">
         <v>-122.63244229199999</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="1">
+      <c r="D36" s="1">
         <v>43.048940233400003</v>
       </c>
-      <c r="D36" s="1">
+      <c r="E36" s="1">
         <v>-115.865880301</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="1">
+      <c r="D37" s="1">
         <v>39.121056975000002</v>
       </c>
-      <c r="D37" s="1">
+      <c r="E37" s="1">
         <v>-121.395465168</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="1">
+      <c r="D38" s="1">
         <v>34.643357994600002</v>
       </c>
-      <c r="D38" s="1">
+      <c r="E38" s="1">
         <v>-77.305104048900006</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="1">
+      <c r="D39" s="1">
         <v>28.233869335000001</v>
       </c>
-      <c r="D39" s="1">
+      <c r="E39" s="1">
         <v>-80.608007519400005</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="1">
+      <c r="D40" s="1">
         <v>31.415160500900001</v>
       </c>
-      <c r="D40" s="1">
+      <c r="E40" s="1">
         <v>-85.4634025079</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="1">
+      <c r="D41" s="1">
         <v>21.4754122511</v>
       </c>
-      <c r="D41" s="1">
+      <c r="E41" s="1">
         <v>-158.03553678399999</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="1">
+      <c r="D42" s="1">
         <v>35.873838181300002</v>
       </c>
-      <c r="D42" s="1">
+      <c r="E42" s="1">
         <v>-88.706128435400004</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="1">
+      <c r="D43" s="1">
         <v>32.675030306899998</v>
       </c>
-      <c r="D43" s="1">
+      <c r="E43" s="1">
         <v>-94.133877756999993</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="1">
+      <c r="D44" s="1">
         <v>34.710463920800002</v>
       </c>
-      <c r="D44" s="1">
+      <c r="E44" s="1">
         <v>-84.165876360499993</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C45" s="1">
+      <c r="D45" s="1">
         <v>39.549253038099998</v>
       </c>
-      <c r="D45" s="1">
+      <c r="E45" s="1">
         <v>-78.845734541400006</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="1">
+      <c r="D46" s="1">
         <v>13.465862204900001</v>
       </c>
-      <c r="D46" s="1">
+      <c r="E46" s="1">
         <v>144.72320415600001</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="1">
+      <c r="D47" s="1">
         <v>47.702713439100002</v>
       </c>
-      <c r="D47" s="1">
+      <c r="E47" s="1">
         <v>-117.577508532</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="1">
+      <c r="D48" s="1">
         <v>32.640615070000003</v>
       </c>
-      <c r="D48" s="1">
+      <c r="E48" s="1">
         <v>-113.055868336</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C49" s="1">
+      <c r="D49" s="1">
         <v>30.5230982285</v>
       </c>
-      <c r="D49" s="1">
+      <c r="E49" s="1">
         <v>-90.412182537000007</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C50" s="1">
+      <c r="D50" s="1">
         <v>33.794439452100001</v>
       </c>
-      <c r="D50" s="1">
+      <c r="E50" s="1">
         <v>-82.277770627199999</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="1">
+      <c r="D51" s="1">
         <v>44.065667941999997</v>
       </c>
-      <c r="D51" s="1">
+      <c r="E51" s="1">
         <v>-122.977783398</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="1">
+      <c r="D52" s="1">
         <v>44.396512026300002</v>
       </c>
-      <c r="D52" s="1">
+      <c r="E52" s="1">
         <v>-70.936540992900007</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="1">
+      <c r="D53" s="1">
         <v>33.773053249100002</v>
       </c>
-      <c r="D53" s="1">
+      <c r="E53" s="1">
         <v>-118.30102733299999</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="1">
+      <c r="D54" s="1">
         <v>32.9489566811</v>
       </c>
-      <c r="D54" s="1">
+      <c r="E54" s="1">
         <v>-115.750656601</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C55" s="1">
+      <c r="D55" s="1">
         <v>18.509432713300001</v>
       </c>
-      <c r="D55" s="1">
+      <c r="E55" s="1">
         <v>-67.099128809700005</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C56" s="1">
+      <c r="D56" s="1">
         <v>37.306397208200003</v>
       </c>
-      <c r="D56" s="1">
+      <c r="E56" s="1">
         <v>-116.198549994</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="1">
+      <c r="D57" s="1">
         <v>31.122537386000001</v>
       </c>
-      <c r="D57" s="1">
+      <c r="E57" s="1">
         <v>-85.979096517200006</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="1">
+      <c r="D58" s="1">
         <v>47.054474053299998</v>
       </c>
-      <c r="D58" s="1">
+      <c r="E58" s="1">
         <v>-122.552700903</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="1">
+      <c r="D59" s="1">
         <v>32.009656509400003</v>
       </c>
-      <c r="D59" s="1">
+      <c r="E59" s="1">
         <v>-81.153560185100005</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C60" s="1">
+      <c r="D60" s="1">
         <v>38.9584020247</v>
       </c>
-      <c r="D60" s="1">
+      <c r="E60" s="1">
         <v>-110.096989229</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="1">
+      <c r="D61" s="1">
         <v>13.4015824973</v>
       </c>
-      <c r="D61" s="1">
+      <c r="E61" s="1">
         <v>144.67867992000001</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C62" s="1">
+      <c r="D62" s="1">
         <v>13.508010198499999</v>
       </c>
-      <c r="D62" s="1">
+      <c r="E62" s="1">
         <v>144.86575904099999</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C63" s="1">
+      <c r="D63" s="1">
         <v>48.123703458199998</v>
       </c>
-      <c r="D63" s="1">
+      <c r="E63" s="1">
         <v>-122.17105604299999</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C64" s="1">
+      <c r="D64" s="1">
         <v>29.1183865271</v>
       </c>
-      <c r="D64" s="1">
+      <c r="E64" s="1">
         <v>-100.47229345</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C65" s="1">
+      <c r="D65" s="1">
         <v>32.962927933300001</v>
       </c>
-      <c r="D65" s="1">
+      <c r="E65" s="1">
         <v>-79.963572477100001</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C66" s="1">
+      <c r="D66" s="1">
         <v>33.538406301000002</v>
       </c>
-      <c r="D66" s="1">
+      <c r="E66" s="1">
         <v>-112.321762273</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C67" s="1">
+      <c r="D67" s="1">
         <v>47.476545603600002</v>
       </c>
-      <c r="D67" s="1">
+      <c r="E67" s="1">
         <v>-111.36497959099999</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C68" s="1">
+      <c r="D68" s="1">
         <v>46.913722407999998</v>
       </c>
-      <c r="D68" s="1">
+      <c r="E68" s="1">
         <v>-96.804464430799996</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C69" s="1">
+      <c r="D69" s="1">
         <v>41.501405282</v>
       </c>
-      <c r="D69" s="1">
+      <c r="E69" s="1">
         <v>-74.084345354800007</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C70" s="1">
+      <c r="D70" s="1">
         <v>44.4744278549</v>
       </c>
-      <c r="D70" s="1">
+      <c r="E70" s="1">
         <v>-73.147896816799999</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C71" s="1">
+      <c r="D71" s="1">
         <v>29.884619396600002</v>
       </c>
-      <c r="D71" s="1">
+      <c r="E71" s="1">
         <v>-98.219381260099993</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C72" s="1">
+      <c r="D72" s="1">
         <v>41.810215159999998</v>
       </c>
-      <c r="D72" s="1">
+      <c r="E72" s="1">
         <v>-93.781302588100004</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C73" s="1">
+      <c r="D73" s="1">
         <v>40.4359467182</v>
       </c>
-      <c r="D73" s="1">
+      <c r="E73" s="1">
         <v>-76.629690458499994</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C74" s="1">
+      <c r="D74" s="1">
         <v>32.864865698499997</v>
       </c>
-      <c r="D74" s="1">
+      <c r="E74" s="1">
         <v>-98.029570797600002</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C75" s="1">
+      <c r="D75" s="1">
         <v>31.439419684000001</v>
       </c>
-      <c r="D75" s="1">
+      <c r="E75" s="1">
         <v>-92.295555911600005</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C76" s="1">
+      <c r="D76" s="1">
         <v>35.339152104900002</v>
       </c>
-      <c r="D76" s="1">
+      <c r="E76" s="1">
         <v>-120.703075007</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C77" s="1">
+      <c r="D77" s="1">
         <v>18.0130410519</v>
       </c>
-      <c r="D77" s="1">
+      <c r="E77" s="1">
         <v>-66.505651578499993</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C78" s="1">
+      <c r="D78" s="1">
         <v>44.471726582199999</v>
       </c>
-      <c r="D78" s="1">
+      <c r="E78" s="1">
         <v>-72.896538843000002</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C79" s="1">
+      <c r="D79" s="1">
         <v>30.416186888199999</v>
       </c>
-      <c r="D79" s="1">
+      <c r="E79" s="1">
         <v>-89.062874432000001</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C80" s="1">
+      <c r="D80" s="1">
         <v>30.2616699455</v>
       </c>
-      <c r="D80" s="1">
+      <c r="E80" s="1">
         <v>-97.294553701599995</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C81" s="1">
+      <c r="D81" s="1">
         <v>38.844875154199997</v>
       </c>
-      <c r="D81" s="1">
+      <c r="E81" s="1">
         <v>-77.014733546599999</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C82" s="1">
+      <c r="D82" s="1">
         <v>21.346299335699999</v>
       </c>
-      <c r="D82" s="1">
+      <c r="E82" s="1">
         <v>-157.922047733</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C83" s="1">
+      <c r="D83" s="1">
         <v>29.831363194600002</v>
       </c>
-      <c r="D83" s="1">
+      <c r="E83" s="1">
         <v>-90.020866789699994</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C84" s="1">
+      <c r="D84" s="1">
         <v>30.625316637499999</v>
       </c>
-      <c r="D84" s="1">
+      <c r="E84" s="1">
         <v>-87.139827523099996</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C85" s="1">
+      <c r="D85" s="1">
         <v>28.428263980499999</v>
       </c>
-      <c r="D85" s="1">
+      <c r="E85" s="1">
         <v>-80.588426761999997</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C86" s="1">
+      <c r="D86" s="1">
         <v>45.72074181</v>
       </c>
-      <c r="D86" s="1">
+      <c r="E86" s="1">
         <v>-119.687435193</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C87" s="1">
+      <c r="D87" s="1">
         <v>47.9883156828</v>
       </c>
-      <c r="D87" s="1">
+      <c r="E87" s="1">
         <v>-122.223175004</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C88" s="1">
+      <c r="D88" s="1">
         <v>48.338637820199999</v>
       </c>
-      <c r="D88" s="1">
+      <c r="E88" s="1">
         <v>-122.661500903</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C89" s="1">
+      <c r="D89" s="1">
         <v>34.632850780399998</v>
       </c>
-      <c r="D89" s="1">
+      <c r="E89" s="1">
         <v>-86.657170102500004</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C90" s="1">
+      <c r="D90" s="1">
         <v>31.567419034</v>
       </c>
-      <c r="D90" s="1">
+      <c r="E90" s="1">
         <v>-110.329649033</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C91" s="1">
+      <c r="D91" s="1">
         <v>31.278607302299999</v>
       </c>
-      <c r="D91" s="1">
+      <c r="E91" s="1">
         <v>-85.714994514400004</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C92" s="1">
+      <c r="D92" s="1">
         <v>31.340385378800001</v>
       </c>
-      <c r="D92" s="1">
+      <c r="E92" s="1">
         <v>-86.091887870999997</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C93" s="1">
+      <c r="D93" s="1">
         <v>21.361878561899999</v>
       </c>
-      <c r="D93" s="1">
+      <c r="E93" s="1">
         <v>-157.911388913</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C94" s="1">
+      <c r="D94" s="1">
         <v>21.5762316637</v>
       </c>
-      <c r="D94" s="1">
+      <c r="E94" s="1">
         <v>-158.19877580299999</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" s="1" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C95" s="1">
+      <c r="D95" s="1">
         <v>37.418771732700002</v>
       </c>
-      <c r="D95" s="1">
+      <c r="E95" s="1">
         <v>-77.447528994999999</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="1" t="s">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C96" s="1">
+      <c r="D96" s="1">
         <v>32.283871230400003</v>
       </c>
-      <c r="D96" s="1">
+      <c r="E96" s="1">
         <v>-84.954843110499993</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C97" s="1">
+      <c r="D97" s="1">
         <v>31.548491370200001</v>
       </c>
-      <c r="D97" s="1">
+      <c r="E97" s="1">
         <v>-81.619987702200007</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C98" s="1">
+      <c r="D98" s="1">
         <v>43.100101113500003</v>
       </c>
-      <c r="D98" s="1">
+      <c r="E98" s="1">
         <v>-76.121099111099994</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="1" t="s">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C99" s="1">
+      <c r="D99" s="1">
         <v>35.403696584099997</v>
       </c>
-      <c r="D99" s="1">
+      <c r="E99" s="1">
         <v>-97.360302781800002</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100" s="1" t="s">
+    <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C100" s="1">
+      <c r="D100" s="1">
         <v>33.981170322899999</v>
       </c>
-      <c r="D100" s="1">
+      <c r="E100" s="1">
         <v>-77.916458672100006</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C101" s="1">
+      <c r="D101" s="1">
         <v>32.500280958200001</v>
       </c>
-      <c r="D101" s="1">
+      <c r="E101" s="1">
         <v>-93.599941340300006</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C102" s="1">
+      <c r="D102" s="1">
         <v>34.3840149372</v>
       </c>
-      <c r="D102" s="1">
+      <c r="E102" s="1">
         <v>-103.321106281</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="C103" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C103" s="1">
+      <c r="D103" s="1">
         <v>34.409191711699997</v>
       </c>
-      <c r="D103" s="1">
+      <c r="E103" s="1">
         <v>-103.328244295</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" s="1" t="s">
+    <row r="104" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="C104" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C104" s="1">
+      <c r="D104" s="1">
         <v>33.715974276499999</v>
       </c>
-      <c r="D104" s="1">
+      <c r="E104" s="1">
         <v>-112.527923384</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" s="1" t="s">
+    <row r="105" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C105" s="1">
+      <c r="D105" s="1">
         <v>30.4107264037</v>
       </c>
-      <c r="D105" s="1">
+      <c r="E105" s="1">
         <v>-89.061208646699995</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" s="1" t="s">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C106" s="1">
+      <c r="D106" s="1">
         <v>44.086293348600002</v>
       </c>
-      <c r="D106" s="1">
+      <c r="E106" s="1">
         <v>-70.282798355099999</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="1" t="s">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="C107" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C107" s="1">
+      <c r="D107" s="1">
         <v>44.809548293900001</v>
       </c>
-      <c r="D107" s="1">
+      <c r="E107" s="1">
         <v>-68.8333959892</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A108" s="1" t="s">
+    <row r="108" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="C108" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C108" s="1">
+      <c r="D108" s="1">
         <v>35.5697139671</v>
       </c>
-      <c r="D108" s="1">
+      <c r="E108" s="1">
         <v>-106.08104196399999</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="1" t="s">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="C109" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C109" s="1">
+      <c r="D109" s="1">
         <v>38.547574332799996</v>
       </c>
-      <c r="D109" s="1">
+      <c r="E109" s="1">
         <v>-75.063301284100007</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" s="1" t="s">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C110" s="1">
+      <c r="D110" s="1">
         <v>47.116716493699997</v>
       </c>
-      <c r="D110" s="1">
+      <c r="E110" s="1">
         <v>-122.56884003</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="1" t="s">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="C111" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C111" s="1">
+      <c r="D111" s="1">
         <v>39.353125887200001</v>
       </c>
-      <c r="D111" s="1">
+      <c r="E111" s="1">
         <v>-81.442110058400004</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A112" s="1" t="s">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="C112" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C112" s="1">
+      <c r="D112" s="1">
         <v>30.318610607499998</v>
       </c>
-      <c r="D112" s="1">
+      <c r="E112" s="1">
         <v>-97.761572058799999</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" s="1" t="s">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="C113" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C113" s="1">
+      <c r="D113" s="1">
         <v>43.761874414700003</v>
       </c>
-      <c r="D113" s="1">
+      <c r="E113" s="1">
         <v>-98.043893422599993</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" s="1" t="s">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C114" s="1">
+      <c r="D114" s="1">
         <v>32.562403152199998</v>
       </c>
-      <c r="D114" s="1">
+      <c r="E114" s="1">
         <v>-117.112009859</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="1" t="s">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C115" s="1">
+      <c r="D115" s="1">
         <v>36.319179647799999</v>
       </c>
-      <c r="D115" s="1">
+      <c r="E115" s="1">
         <v>-119.93398605</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" s="1" t="s">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="C116" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C116" s="1">
+      <c r="D116" s="1">
         <v>32.724696303499996</v>
       </c>
-      <c r="D116" s="1">
+      <c r="E116" s="1">
         <v>-117.21843191799999</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" s="1" t="s">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="C117" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C117" s="1">
+      <c r="D117" s="1">
         <v>38.4161872655</v>
       </c>
-      <c r="D117" s="1">
+      <c r="E117" s="1">
         <v>-90.398607995899994</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="1" t="s">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="C118" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C118" s="1">
+      <c r="D118" s="1">
         <v>36.269205170900001</v>
       </c>
-      <c r="D118" s="1">
+      <c r="E118" s="1">
         <v>-114.98483901</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="1" t="s">
+    <row r="119" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="C119" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C119" s="1">
+      <c r="D119" s="1">
         <v>47.5555933853</v>
       </c>
-      <c r="D119" s="1">
+      <c r="E119" s="1">
         <v>-122.652356505</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" s="1" t="s">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="C120" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C120" s="1">
+      <c r="D120" s="1">
         <v>37.249439618399997</v>
       </c>
-      <c r="D120" s="1">
+      <c r="E120" s="1">
         <v>-77.334727720199993</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="1" t="s">
+    <row r="121" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="C121" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C121" s="1">
+      <c r="D121" s="1">
         <v>40.699640196600001</v>
       </c>
-      <c r="D121" s="1">
+      <c r="E121" s="1">
         <v>-84.132889403199997</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122" s="1" t="s">
+    <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="C122" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C122" s="1">
+      <c r="D122" s="1">
         <v>32.739958394799999</v>
       </c>
-      <c r="D122" s="1">
+      <c r="E122" s="1">
         <v>-96.956440361099993</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A123" s="1" t="s">
+    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="C123" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C123" s="1">
+      <c r="D123" s="1">
         <v>21.439627444900001</v>
       </c>
-      <c r="D123" s="1">
+      <c r="E123" s="1">
         <v>-158.00310994200001</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="1" t="s">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="C124" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C124" s="1">
+      <c r="D124" s="1">
         <v>36.9433080035</v>
       </c>
-      <c r="D124" s="1">
+      <c r="E124" s="1">
         <v>-76.301513692100002</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" s="1" t="s">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="C125" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C125" s="1">
+      <c r="D125" s="1">
         <v>38.145841636</v>
       </c>
-      <c r="D125" s="1">
+      <c r="E125" s="1">
         <v>-76.427890986700007</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A126" s="1" t="s">
+    <row r="126" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="C126" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C126" s="1">
+      <c r="D126" s="1">
         <v>38.891840041999998</v>
       </c>
-      <c r="D126" s="1">
+      <c r="E126" s="1">
         <v>-123.54657913600001</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A127" s="1" t="s">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="C127" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C127" s="1">
+      <c r="D127" s="1">
         <v>33.917408651300001</v>
       </c>
-      <c r="D127" s="1">
+      <c r="E127" s="1">
         <v>-84.519236218700001</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A128" s="1" t="s">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="C128" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C128" s="1">
+      <c r="D128" s="1">
         <v>33.641312087300001</v>
       </c>
-      <c r="D128" s="1">
+      <c r="E128" s="1">
         <v>-88.451118752100001</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129" s="1" t="s">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="C129" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C129" s="1">
+      <c r="D129" s="1">
         <v>44.817567381499998</v>
       </c>
-      <c r="D129" s="1">
+      <c r="E129" s="1">
         <v>-68.829801382100001</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A130" s="1" t="s">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="C130" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C130" s="1">
+      <c r="D130" s="1">
         <v>35.8114939421</v>
       </c>
-      <c r="D130" s="1">
+      <c r="E130" s="1">
         <v>-84.003670953300002</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A131" s="1" t="s">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="C131" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C131" s="1">
+      <c r="D131" s="1">
         <v>42.941045621699999</v>
       </c>
-      <c r="D131" s="1">
+      <c r="E131" s="1">
         <v>-87.887984283700007</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A132" s="1" t="s">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="C132" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C132" s="1">
+      <c r="D132" s="1">
         <v>42.315260772599999</v>
       </c>
-      <c r="D132" s="1">
+      <c r="E132" s="1">
         <v>-85.251765022599997</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133" s="1" t="s">
+    <row r="133" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="C133" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C133" s="1">
+      <c r="D133" s="1">
         <v>41.365115238000001</v>
       </c>
-      <c r="D133" s="1">
+      <c r="E133" s="1">
         <v>-72.271988326499994</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A134" s="1" t="s">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="C134" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C134" s="1">
+      <c r="D134" s="1">
         <v>29.961082025900001</v>
       </c>
-      <c r="D134" s="1">
+      <c r="E134" s="1">
         <v>-90.005460036900004</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A135" s="1" t="s">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="C135" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C135" s="1">
+      <c r="D135" s="1">
         <v>39.578959641399997</v>
       </c>
-      <c r="D135" s="1">
+      <c r="E135" s="1">
         <v>-85.811023646500004</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136" s="1" t="s">
+    <row r="136" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="C136" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C136" s="1">
+      <c r="D136" s="1">
         <v>41.197178710099998</v>
       </c>
-      <c r="D136" s="1">
+      <c r="E136" s="1">
         <v>-81.084834317399995</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A137" s="1" t="s">
+    <row r="137" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="C137" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C137" s="1">
+      <c r="D137" s="1">
         <v>43.996953370900002</v>
       </c>
-      <c r="D137" s="1">
+      <c r="E137" s="1">
         <v>-92.431667563999994</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A138" s="1" t="s">
+    <row r="138" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="C138" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C138" s="1">
+      <c r="D138" s="1">
         <v>43.2374990056</v>
       </c>
-      <c r="D138" s="1">
+      <c r="E138" s="1">
         <v>-78.972691388499996</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A139" s="1" t="s">
+    <row r="139" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="C139" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C139" s="1">
+      <c r="D139" s="1">
         <v>44.509890214599999</v>
       </c>
-      <c r="D139" s="1">
+      <c r="E139" s="1">
         <v>-73.163556475600004</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" s="1" t="s">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="C140" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C140" s="1">
+      <c r="D140" s="1">
         <v>44.080138702299998</v>
       </c>
-      <c r="D140" s="1">
+      <c r="E140" s="1">
         <v>-103.266957925</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A141" s="1" t="s">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="C141" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C141" s="1">
+      <c r="D141" s="1">
         <v>22.039026069199998</v>
       </c>
-      <c r="D141" s="1">
+      <c r="E141" s="1">
         <v>-159.754233043</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A142" s="1" t="s">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="C142" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C142" s="1">
+      <c r="D142" s="1">
         <v>21.336565761599999</v>
       </c>
-      <c r="D142" s="1">
+      <c r="E142" s="1">
         <v>-157.947911019</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A143" s="1" t="s">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="C143" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C143" s="1">
+      <c r="D143" s="1">
         <v>18.096254399599999</v>
       </c>
-      <c r="D143" s="1">
+      <c r="E143" s="1">
         <v>-65.512251581399994</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A144" s="1" t="s">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="C144" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C144" s="1">
+      <c r="D144" s="1">
         <v>24.564687961000001</v>
       </c>
-      <c r="D144" s="1">
+      <c r="E144" s="1">
         <v>-81.7912167283</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145" s="1" t="s">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="C145" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C145" s="1">
+      <c r="D145" s="1">
         <v>33.994957183799997</v>
       </c>
-      <c r="D145" s="1">
+      <c r="E145" s="1">
         <v>-119.63349683600001</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A146" s="1" t="s">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="C146" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C146" s="1">
+      <c r="D146" s="1">
         <v>13.517951387</v>
       </c>
-      <c r="D146" s="1">
+      <c r="E146" s="1">
         <v>144.811096236</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A147" s="1" t="s">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="C147" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C147" s="1">
+      <c r="D147" s="1">
         <v>31.230999383299999</v>
       </c>
-      <c r="D147" s="1">
+      <c r="E147" s="1">
         <v>-85.650634717800003</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A148" s="1" t="s">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="C148" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C148" s="1">
+      <c r="D148" s="1">
         <v>31.815733182199999</v>
       </c>
-      <c r="D148" s="1">
+      <c r="E148" s="1">
         <v>-85.649798495699997</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A149" s="1" t="s">
+    <row r="149" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="C149" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C149" s="1">
+      <c r="D149" s="1">
         <v>33.159463674199998</v>
       </c>
-      <c r="D149" s="1">
+      <c r="E149" s="1">
         <v>-106.425696182</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A150" s="1" t="s">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="C150" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C150" s="1">
+      <c r="D150" s="1">
         <v>37.013020396199998</v>
       </c>
-      <c r="D150" s="1">
+      <c r="E150" s="1">
         <v>-76.304376054399995</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A151" s="1" t="s">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="C151" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C151" s="1">
+      <c r="D151" s="1">
         <v>21.386628486900001</v>
       </c>
-      <c r="D151" s="1">
+      <c r="E151" s="1">
         <v>-157.90564130800001</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A152" s="1" t="s">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="C152" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C152" s="1">
+      <c r="D152" s="1">
         <v>21.362146270299998</v>
       </c>
-      <c r="D152" s="1">
+      <c r="E152" s="1">
         <v>-157.71826608200001</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A153" s="1" t="s">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="C153" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C153" s="1">
+      <c r="D153" s="1">
         <v>42.091733208299999</v>
       </c>
-      <c r="D153" s="1">
+      <c r="E153" s="1">
         <v>-87.836545041999997</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A154" s="1" t="s">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B154" s="1" t="s">
+      <c r="C154" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C154" s="1">
+      <c r="D154" s="1">
         <v>27.896530459299999</v>
       </c>
-      <c r="D154" s="1">
+      <c r="E154" s="1">
         <v>-98.043430722500005</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A155" s="1" t="s">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B155" s="1" t="s">
+      <c r="C155" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C155" s="1">
+      <c r="D155" s="1">
         <v>38.6628404569</v>
       </c>
-      <c r="D155" s="1">
+      <c r="E155" s="1">
         <v>-121.403205934</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A156" s="1" t="s">
+    <row r="156" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B156" s="1" t="s">
+      <c r="C156" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C156" s="1">
+      <c r="D156" s="1">
         <v>42.740232967499999</v>
       </c>
-      <c r="D156" s="1">
+      <c r="E156" s="1">
         <v>-115.563336812</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A157" s="1" t="s">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B157" s="1" t="s">
+      <c r="C157" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C157" s="1">
+      <c r="D157" s="1">
         <v>29.3567318395</v>
       </c>
-      <c r="D157" s="1">
+      <c r="E157" s="1">
         <v>-100.782932919</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A158" s="1" t="s">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B158" s="1" t="s">
+      <c r="C158" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C158" s="1">
+      <c r="D158" s="1">
         <v>39.706672895899999</v>
       </c>
-      <c r="D158" s="1">
+      <c r="E158" s="1">
         <v>-104.757676168</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A159" s="1" t="s">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B159" s="1" t="s">
+      <c r="C159" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C159" s="1">
+      <c r="D159" s="1">
         <v>30.045471201200002</v>
       </c>
-      <c r="D159" s="1">
+      <c r="E159" s="1">
         <v>-85.551368886199995</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A160" s="1" t="s">
+    <row r="160" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B160" s="1" t="s">
+      <c r="C160" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C160" s="1">
+      <c r="D160" s="1">
         <v>32.9398358551</v>
       </c>
-      <c r="D160" s="1">
+      <c r="E160" s="1">
         <v>-88.579142625599999</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A161" s="1" t="s">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="C161" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C161" s="1">
+      <c r="D161" s="1">
         <v>31.432178155700001</v>
       </c>
-      <c r="D161" s="1">
+      <c r="E161" s="1">
         <v>-100.404389232</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A162" s="1" t="s">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="C162" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C162" s="1">
+      <c r="D162" s="1">
         <v>61.2656445617</v>
       </c>
-      <c r="D162" s="1">
+      <c r="E162" s="1">
         <v>-149.64102546800001</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A163" s="1" t="s">
+    <row r="163" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B163" s="1" t="s">
+      <c r="C163" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C163" s="1">
+      <c r="D163" s="1">
         <v>64.317537766699999</v>
       </c>
-      <c r="D163" s="1">
+      <c r="E163" s="1">
         <v>-146.64698092899999</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A164" t="s">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164" t="s">
         <v>210</v>
       </c>
-      <c r="B164" s="1" t="s">
+      <c r="C164" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C164">
+      <c r="D164">
         <v>33.315199999999997</v>
       </c>
-      <c r="D164">
+      <c r="E164">
         <v>44.366100000000003</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A165" s="1" t="s">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="C165" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C165">
+      <c r="D165">
         <v>38.907200000000003</v>
       </c>
-      <c r="D165">
+      <c r="E165">
         <v>-77.036900000000003</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A166" t="s">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166" t="s">
         <v>215</v>
       </c>
-      <c r="B166" t="s">
+      <c r="C166" t="s">
         <v>214</v>
       </c>
-      <c r="C166" s="2">
+      <c r="D166" s="2">
         <v>-23.37</v>
       </c>
-      <c r="D166">
+      <c r="E166">
         <v>-132.34</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A167" s="1" t="s">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="C167" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C167">
+      <c r="D167">
         <v>16.9742</v>
       </c>
-      <c r="D167">
+      <c r="E167">
         <v>-7.9865000000000004</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A168" t="s">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" t="s">
         <v>218</v>
       </c>
-      <c r="B168" t="s">
+      <c r="C168" t="s">
         <v>219</v>
       </c>
-      <c r="C168">
+      <c r="D168">
         <v>48.775799999999997</v>
       </c>
-      <c r="D168">
+      <c r="E168">
         <v>-9.1829000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new military bases
</commit_message>
<xml_diff>
--- a/MilitaryBases.xlsx
+++ b/MilitaryBases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshs\Documents\Arsh Files on PC\Virginia Tech\Year 1\Semester 2\Clubs\WebDVT\HTML\html-cheat-sheet\TheSunNeverSetsOnTheAmericanMilitaryBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD68627-5863-4756-943C-5E96F29AC61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02F941F-7072-426A-B903-A2BBE0B513AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="834" yWindow="-96" windowWidth="22302" windowHeight="14592" xr2:uid="{E398A702-D2C5-4257-8B81-705240FEDC0C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="237">
   <si>
     <t>NG Springfield AVCRAD (New)</t>
   </si>
@@ -682,9 +682,6 @@
     <t>Northern Territory</t>
   </si>
   <si>
-    <t>Alice Springs</t>
-  </si>
-  <si>
     <t>Niger</t>
   </si>
   <si>
@@ -704,6 +701,51 @@
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>Pine Gap (Alice Springs)</t>
+  </si>
+  <si>
+    <t>Naval Communication Station Harold E. Holt</t>
+  </si>
+  <si>
+    <t>Exmouth, Western Australia</t>
+  </si>
+  <si>
+    <t>Al-Harir Air Base</t>
+  </si>
+  <si>
+    <t>Harir, Kurdistan Region, Iraq</t>
+  </si>
+  <si>
+    <t>Aytos Logistics Center</t>
+  </si>
+  <si>
+    <t>Aytos, Bulgaria</t>
+  </si>
+  <si>
+    <t>Caserma Ederle</t>
+  </si>
+  <si>
+    <t>Vicenza, Italy</t>
+  </si>
+  <si>
+    <t>Misawa Air Base</t>
+  </si>
+  <si>
+    <t>Misawa, Aomori</t>
+  </si>
+  <si>
+    <t>Camp Bondsteel</t>
+  </si>
+  <si>
+    <t>Ferizaj, Kosovo</t>
+  </si>
+  <si>
+    <t>Naval Air Station Keflavik</t>
+  </si>
+  <si>
+    <t>Keflavik International Airport, Iceland</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCADE206-E22A-485D-8E8A-6C74ACC938AD}">
-  <dimension ref="A1:E168"/>
+  <dimension ref="A1:E175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168:A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1084,7 +1126,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B1" t="s">
         <v>208</v>
@@ -1093,10 +1135,10 @@
         <v>209</v>
       </c>
       <c r="D1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E1" t="s">
         <v>220</v>
-      </c>
-      <c r="E1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3892,7 +3934,7 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="C166" t="s">
         <v>214</v>
@@ -3909,10 +3951,10 @@
         <v>166</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D167">
         <v>16.9742</v>
@@ -3926,16 +3968,135 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
+        <v>217</v>
+      </c>
+      <c r="C168" t="s">
         <v>218</v>
-      </c>
-      <c r="C168" t="s">
-        <v>219</v>
       </c>
       <c r="D168">
         <v>48.775799999999997</v>
       </c>
       <c r="E168">
         <v>-9.1829000000000001</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169" t="s">
+        <v>223</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D169">
+        <v>-21.485900000000001</v>
+      </c>
+      <c r="E169">
+        <v>114.0956</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" t="s">
+        <v>225</v>
+      </c>
+      <c r="C170" t="s">
+        <v>226</v>
+      </c>
+      <c r="D170">
+        <v>36.313699999999997</v>
+      </c>
+      <c r="E170">
+        <v>44.305</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171" t="s">
+        <v>227</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D171">
+        <v>42.424100000000003</v>
+      </c>
+      <c r="E171">
+        <v>27.1358</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
+        <v>229</v>
+      </c>
+      <c r="C172" t="s">
+        <v>230</v>
+      </c>
+      <c r="D172">
+        <v>45.323270000000001</v>
+      </c>
+      <c r="E172">
+        <v>11.344262000000001</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173" t="s">
+        <v>231</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D173">
+        <v>40.421900000000001</v>
+      </c>
+      <c r="E173">
+        <v>141.22190000000001</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174" t="s">
+        <v>233</v>
+      </c>
+      <c r="C174" t="s">
+        <v>234</v>
+      </c>
+      <c r="D174">
+        <v>42.2194</v>
+      </c>
+      <c r="E174">
+        <v>21.149000000000001</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175" t="s">
+        <v>235</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D175">
+        <v>63.590600000000002</v>
+      </c>
+      <c r="E175">
+        <v>22.361999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>